<commit_message>
versão de entrega na plataforma
</commit_message>
<xml_diff>
--- a/candidatos_linkedin_unnested_sent.xlsx
+++ b/candidatos_linkedin_unnested_sent.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="68" documentId="8_{6ABC28EE-E991-4A70-A4EC-92CEEDEAA36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{856EA58A-EAB6-470C-A136-18C1EE7C6FD0}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="3360" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{3BB47F79-0CA3-4A22-B364-90F6E6EA3EAB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{3BB47F79-0CA3-4A22-B364-90F6E6EA3EAB}"/>
   </bookViews>
   <sheets>
     <sheet name="candidatos_linkedin_unnested_se" sheetId="2" r:id="rId1"/>
@@ -1734,6 +1734,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{6FD4BFCD-B04D-4968-AA90-9FFC178B238B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="8" unboundColumnsRight="1">
@@ -21387,9 +21391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B814685-2A54-44CD-8AAB-48CA76FE7E12}">
   <dimension ref="A1:L159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection sqref="A1:L1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>